<commit_message>
Checkpoint before assistant change: Improve visibility of results by adjusting contrast for better readability
Modify contrast settings in glaucoma_test_results.xlsx to enhance visual clarity.

Replit-Commit-Author: Assistant
</commit_message>
<xml_diff>
--- a/glaucoma_test_results.xlsx
+++ b/glaucoma_test_results.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -500,6 +500,51 @@
         <is>
           <t>Defects Detected</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>ANI</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2025-05-27T09:31:45.432Z</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2025-05-27T09:32:59.486Z</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>74</v>
+      </c>
+      <c r="F2" t="n">
+        <v>48</v>
+      </c>
+      <c r="G2" t="n">
+        <v>22</v>
+      </c>
+      <c r="H2" t="n">
+        <v>45.83</v>
+      </c>
+      <c r="J2" t="n">
+        <v>48</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>[{'pointIndex': 0, 'row': 0, 'col': 5, 'detected': True, 'reactionTime': 2632, 'timestamp': '2025-05-27T09:31:48.064Z'}, {'pointIndex': 1, 'row': 2, 'col': 5, 'detected': True, 'reactionTime': 1368, 'timestamp': '2025-05-27T09:31:49.944Z'}, {'pointIndex': 2, 'row': 2, 'col': 0, 'detected': False, 'reactionTime': 3000, 'timestamp': '2025-05-27T09:31:53.453Z'}, {'pointIndex': 3, 'row': 1, 'col': 6, 'detected': True, 'reactionTime': 1784, 'timestamp': '2025-05-27T09:31:55.746Z'}, {'pointIndex': 4, 'row': 5, 'col': 4, 'detected': True, 'reactionTime': 1856, 'timestamp': '2025-05-27T09:31:58.118Z'}, {'pointIndex': 5, 'row': 4, 'col': 3, 'detected': True, 'reactionTime': 1200, 'timestamp': '2025-05-27T09:31:59.831Z'}, {'pointIndex': 6, 'row': 0, 'col': 2, 'detected': True, 'reactionTime': 1316, 'timestamp': '2025-05-27T09:32:01.649Z'}, {'pointIndex': 7, 'row': 1, 'col': 1, 'detected': True, 'reactionTime': 1185, 'timestamp': '2025-05-27T09:32:03.344Z'}, {'pointIndex': 8, 'row': 3, 'col': 0, 'detected': True, 'reactionTime': 2535, 'timestamp': '2025-05-27T09:32:06.383Z'}, {'pointIndex': 9, 'row': 4, 'col': 6, 'detected': True, 'reactionTime': 1928, 'timestamp': '2025-05-27T09:32:08.816Z'}, {'pointIndex': 10, 'row': 1, 'col': 3, 'detected': True, 'reactionTime': 1656, 'timestamp': '2025-05-27T09:32:10.983Z'}, {'pointIndex': 11, 'row': 5, 'col': 2, 'detected': True, 'reactionTime': 1385, 'timestamp': '2025-05-27T09:32:12.883Z'}, {'pointIndex': 12, 'row': 1, 'col': 2, 'detected': True, 'reactionTime': 1139, 'timestamp': '2025-05-27T09:32:14.533Z'}, {'pointIndex': 13, 'row': 2, 'col': 7, 'detected': True, 'reactionTime': 1669, 'timestamp': '2025-05-27T09:32:16.714Z'}, {'pointIndex': 14, 'row': 1, 'col': 5, 'detected': True, 'reactionTime': 1116, 'timestamp': '2025-05-27T09:32:18.332Z'}, {'pointIndex': 15, 'row': 0, 'col': 5, 'detected': True, 'reactionTime': 1957, 'timestamp': '2025-05-27T09:32:20.799Z'}, {'pointIndex': 16, 'row': 5, 'col': 0, 'detected': True, 'reactionTime': 1701, 'timestamp': '2025-05-27T09:32:23.012Z'}, {'pointIndex': 17, 'row': 0, 'col': 1, 'detected': True, 'reactionTime': 1619, 'timestamp': '2025-05-27T09:32:25.131Z'}, {'pointIndex': 18, 'row': 4, 'col': 7, 'detected': True, 'reactionTime': 1590, 'timestamp': '2025-05-27T09:32:27.235Z'}, {'pointIndex': 19, 'row': 3, 'col': 5, 'detected': True, 'reactionTime': 1267, 'timestamp': '2025-05-27T09:32:29.018Z'}, {'pointIndex': 20, 'row': 3, 'col': 0, 'detected': False, 'reactionTime': 3000, 'timestamp': '2025-05-27T09:32:30.385Z'}, {'pointIndex': 21, 'row': 0, 'col': 2, 'detected': False, 'reactionTime': 3000, 'timestamp': '2025-05-27T09:32:30.940Z'}, {'pointIndex': 22, 'row': 5, 'col': 7, 'detected': False, 'reactionTime': 3000, 'timestamp': '2025-05-27T09:32:31.488Z'}, {'pointIndex': 23, 'row': 3, 'col': 2, 'detected': False, 'reactionTime': 3000, 'timestamp': '2025-05-27T09:32:32.101Z'}, {'pointIndex': 24, 'row': 2, 'col': 2, 'detected': False, 'reactionTime': 3000, 'timestamp': '2025-05-27T09:32:32.998Z'}, {'pointIndex': 25, 'row': 2, 'col': 7, 'detected': False, 'reactionTime': 3000, 'timestamp': '2025-05-27T09:32:33.640Z'}, {'pointIndex': 26, 'row': 0, 'col': 1, 'detected': False, 'reactionTime': 3000, 'timestamp': '2025-05-27T09:32:34.353Z'}, {'pointIndex': 27, 'row': 1, 'col': 6, 'detected': False, 'reactionTime': 3000, 'timestamp': '2025-05-27T09:32:37.882Z'}, {'pointIndex': 28, 'row': 5, 'col': 3, 'detected': True, 'reactionTime': 1304, 'timestamp': '2025-05-27T09:32:39.701Z'}, {'pointIndex': 29, 'row': 0, 'col': 3, 'detected': False, 'reactionTime': 3000, 'timestamp': '2025-05-27T09:32:40.707Z'}, {'pointIndex': 30, 'row': 2, 'col': 0, 'detected': False, 'reactionTime': 3000, 'timestamp': '2025-05-27T09:32:41.305Z'}, {'pointIndex': 31, 'row': 4, 'col': 3, 'detected': False, 'reactionTime': 3000, 'timestamp': '2025-05-27T09:32:41.882Z'}, {'pointIndex': 32, 'row': 5, 'col': 0, 'detected': False, 'reactionTime': 3000, 'timestamp': '2025-05-27T09:32:42.745Z'}, {'pointIndex': 33, 'row': 2, 'col': 5, 'detected': False, 'reactionTime': 3000, 'timestamp': '2025-05-27T09:32:43.322Z'}, {'pointIndex': 34, 'row': 1, 'col': 0, 'detected': False, 'reactionTime': 3000, 'timestamp': '2025-05-27T09:32:43.907Z'}, {'pointIndex': 35, 'row': 1, 'col': 5, 'detected': False, 'reactionTime': 3000, 'timestamp': '2025-05-27T09:32:44.448Z'}, {'pointIndex': 36, 'row': 4, 'col': 5, 'detected': False, 'reactionTime': 3000, 'timestamp': '2025-05-27T09:32:45.090Z'}, {'pointIndex': 37, 'row': 3, 'col': 3, 'detected': False, 'reactionTime': 3000, 'timestamp': '2025-05-27T09:32:45.746Z'}, {'pointIndex': 38, 'row': 5, 'col': 1, 'detected': False, 'reactionTime': 3000, 'timestamp': '2025-05-27T09:32:46.407Z'}, {'pointIndex': 39, 'row': 1, 'col': 5, 'detected': True, 'reactionTime': 1789, 'timestamp': '2025-05-27T09:32:48.703Z'}, {'pointIndex': 40, 'row': 5, 'col': 7, 'detected': True, 'reactionTime': 1444, 'timestamp': '2025-05-27T09:32:50.653Z'}, {'pointIndex': 41, 'row': 0, 'col': 7, 'detected': False, 'reactionTime': 921, 'timestamp': '2025-05-27T09:32:52.081Z'}, {'pointIndex': 42, 'row': 1, 'col': 5, 'detected': False, 'reactionTime': 857, 'timestamp': '2025-05-27T09:32:53.439Z'}, {'pointIndex': 43, 'row': 3, 'col': 1, 'detected': False, 'reactionTime': 524, 'timestamp': '2025-05-27T09:32:54.470Z'}, {'pointIndex': 44, 'row': 0, 'col': 0, 'detected': False, 'reactionTime': 701, 'timestamp': '2025-05-27T09:32:55.684Z'}, {'pointIndex': 45, 'row': 2, 'col': 6, 'detected': False, 'reactionTime': 3000, 'timestamp': '2025-05-27T09:32:57.621Z'}, {'pointIndex': 46, 'row': 3, 'col': 5, 'detected': False, 'reactionTime': 3000, 'timestamp': '2025-05-27T09:32:58.299Z'}, {'pointIndex': 47, 'row': 5, 'col': 0, 'detected': False, 'reactionTime': 3000, 'timestamp': '2025-05-27T09:32:58.983Z'}]</t>
+        </is>
+      </c>
+      <c r="L2" t="n">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -513,7 +558,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -581,6 +626,53 @@
         <is>
           <t>Letter Accuracy</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>ANI</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2025-05-27T09:33:55.020Z</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2025-05-27T09:34:38.943Z</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>44</v>
+      </c>
+      <c r="F2" t="n">
+        <v>20</v>
+      </c>
+      <c r="G2" t="n">
+        <v>12</v>
+      </c>
+      <c r="H2" t="n">
+        <v>60</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>English</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>[100, 50, 25, 12.5, 6.25, 3.125, 1.56, 0.78, 0.39, 0.195]</t>
+        </is>
+      </c>
+      <c r="L2" t="n">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -807,7 +899,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -875,6 +967,40 @@
         <is>
           <t>Log Units</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>ANI</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2025-05-27T09:35:34.132Z</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2025-05-27T09:38:55.761Z</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>202</v>
+      </c>
+      <c r="F2" t="n">
+        <v>40</v>
+      </c>
+      <c r="G2" t="n">
+        <v>16</v>
+      </c>
+      <c r="H2" t="n">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Checkpoint before assistant change: Update glaucoma test result data with the latest patient information
Update glaucoma_test_results.xlsx with new patient data.

Replit-Commit-Author: Assistant
</commit_message>
<xml_diff>
--- a/glaucoma_test_results.xlsx
+++ b/glaucoma_test_results.xlsx
@@ -558,7 +558,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -673,6 +673,53 @@
       </c>
       <c r="L2" t="n">
         <v>12</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ANI</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2025-05-27T15:09:35.311Z</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2025-05-27T15:10:04.946Z</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>30</v>
+      </c>
+      <c r="F3" t="n">
+        <v>20</v>
+      </c>
+      <c r="G3" t="n">
+        <v>13</v>
+      </c>
+      <c r="H3" t="n">
+        <v>65</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>English</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>[100, 50, 25, 12.5, 6.25, 3.125, 1.56, 0.78, 0.39, 0.195]</t>
+        </is>
+      </c>
+      <c r="L3" t="n">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -899,7 +946,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1001,6 +1048,52 @@
       </c>
       <c r="H2" t="n">
         <v>40</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ANI</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>8:42:20 PM</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>8:44:21 PM</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>121</v>
+      </c>
+      <c r="F3" t="n">
+        <v>72</v>
+      </c>
+      <c r="G3" t="n">
+        <v>72</v>
+      </c>
+      <c r="H3" t="n">
+        <v>100</v>
+      </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>english</t>
+        </is>
+      </c>
+      <c r="K3" t="n">
+        <v>1.15</v>
+      </c>
+      <c r="L3" t="n">
+        <v>1.15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated project: Glaucoma test app with full features
</commit_message>
<xml_diff>
--- a/glaucoma_test_results.xlsx
+++ b/glaucoma_test_results.xlsx
@@ -946,7 +946,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1083,7 +1083,6 @@
       <c r="H3" t="n">
         <v>100</v>
       </c>
-      <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr">
         <is>
           <t>english</t>
@@ -1093,6 +1092,51 @@
         <v>1.15</v>
       </c>
       <c r="L3" t="n">
+        <v>1.15</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ANI</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>8:51:46 PM</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>8:52:40 PM</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>54</v>
+      </c>
+      <c r="F4" t="n">
+        <v>72</v>
+      </c>
+      <c r="G4" t="n">
+        <v>72</v>
+      </c>
+      <c r="H4" t="n">
+        <v>100</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>english</t>
+        </is>
+      </c>
+      <c r="K4" t="n">
+        <v>1.15</v>
+      </c>
+      <c r="L4" t="n">
         <v>1.15</v>
       </c>
     </row>

</xml_diff>